<commit_message>
Fixed via issues on PCB
</commit_message>
<xml_diff>
--- a/Docs/BOM_Group_3.xlsx
+++ b/Docs/BOM_Group_3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b1fd496a47fa4da2/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\adrian\EEE3088F\EEE3088F-Group-3\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7E4635B-8BB2-477D-A902-A2534B6DE58B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518FE60D-8B9F-43E1-8AFB-C887289E10A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="15390" windowHeight="13500" xr2:uid="{26469A26-CE12-476E-91B8-81E814CF6A42}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{26469A26-CE12-476E-91B8-81E814CF6A42}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -632,10 +632,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="&quot;R&quot;#,##0;[Red]\-&quot;R&quot;#,##0"/>
-    <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="6" formatCode="&quot;R&quot;#,##0;[Red]\-&quot;R&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1258,7 +1258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="42" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1267,7 +1267,7 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1290,12 +1290,13 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1308,7 +1309,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1667,11 +1667,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C604B193-2981-424E-9BAA-D7E15C8CB1A8}">
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16:Q21"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="132" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
@@ -1688,7 +1688,7 @@
     <col min="22" max="22" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30">
+    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="16.5">
+    <row r="2" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>12</v>
       </c>
@@ -1766,12 +1766,12 @@
         <f>K2+3*C2</f>
         <v>2.3E-2</v>
       </c>
-      <c r="P2" s="28" t="s">
+      <c r="P2" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="28"/>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="Q2" s="29"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>18</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>3.6037999899999997</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>24</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>18.018999949999998</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>30</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>34</v>
       </c>
@@ -1948,12 +1948,12 @@
         <f t="shared" si="2"/>
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="P6" s="31" t="s">
+      <c r="P6" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="Q6" s="31"/>
-    </row>
-    <row r="7" spans="1:17" ht="16.5">
+      <c r="Q6" s="32"/>
+    </row>
+    <row r="7" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>39</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>3.5442</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>44</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>17.721</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="32.25" customHeight="1">
+    <row r="9" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>49</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>3.3374999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>53</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>1.9999949999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="60">
+    <row r="11" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>58</v>
       </c>
@@ -2171,12 +2171,12 @@
         <f t="shared" si="2"/>
         <v>0.13200000000000001</v>
       </c>
-      <c r="P11" s="30" t="s">
+      <c r="P11" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="Q11" s="30"/>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="Q11" s="31"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P12" s="3" t="s">
         <v>23</v>
       </c>
@@ -2185,16 +2185,16 @@
         <v>1.2916666600000002</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P13" s="3" t="s">
         <v>29</v>
       </c>
       <c r="Q13" s="24">
         <f>SUM(L15:L31)</f>
-        <v>6.4583333000000014</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="30.75">
+        <v>9.4583333000000014</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>0</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>64</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>0.87999999999999989</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>69</v>
       </c>
@@ -2315,12 +2315,12 @@
         <f>K16+3*C16</f>
         <v>2.3E-2</v>
       </c>
-      <c r="P16" s="29" t="s">
+      <c r="P16" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="Q16" s="29"/>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="Q16" s="30"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>74</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>18.018999949999998</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>80</v>
       </c>
@@ -2415,10 +2415,10 @@
       </c>
       <c r="Q18" s="24">
         <f>Q13</f>
-        <v>6.4583333000000014</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="30.75">
+        <v>9.4583333000000014</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>53</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>17.721</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>58</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="16.5">
+    <row r="21" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
         <v>90</v>
       </c>
@@ -2561,10 +2561,10 @@
       </c>
       <c r="Q21" s="27">
         <f>SUM(Q17:Q20)</f>
-        <v>54.198333250000005</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="16.5">
+        <v>57.198333250000005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
         <v>90</v>
       </c>
@@ -2607,14 +2607,16 @@
       </c>
       <c r="Q22" s="6"/>
     </row>
-    <row r="23" spans="1:17" ht="16.5">
+    <row r="23" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
         <v>99</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
       <c r="D23" s="4" t="s">
         <v>101</v>
       </c>
@@ -2644,18 +2646,20 @@
       </c>
       <c r="L23" s="2">
         <f>K23+3*C23</f>
-        <v>5.1500000000000004E-2</v>
+        <v>3.0514999999999999</v>
       </c>
       <c r="Q23" s="6"/>
     </row>
-    <row r="24" spans="1:17" ht="16.5">
+    <row r="24" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
         <v>104</v>
       </c>
       <c r="B24" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="2">
+        <v>0</v>
+      </c>
       <c r="D24" s="4" t="s">
         <v>106</v>
       </c>
@@ -2689,7 +2693,7 @@
       </c>
       <c r="Q24" s="6"/>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>109</v>
       </c>
@@ -2731,7 +2735,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>114</v>
       </c>
@@ -2773,7 +2777,7 @@
         <v>1.62</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>119</v>
       </c>
@@ -2815,7 +2819,7 @@
         <v>1.4000000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>124</v>
       </c>
@@ -2857,7 +2861,7 @@
         <v>0.24199999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>128</v>
       </c>
@@ -2899,7 +2903,7 @@
         <v>0.48199999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>133</v>
       </c>
@@ -2941,7 +2945,7 @@
         <v>0.39849999999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>137</v>
       </c>
@@ -2983,7 +2987,7 @@
         <v>1.0135000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="30">
+    <row r="33" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>0</v>
       </c>
@@ -3021,7 +3025,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="30">
+    <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>143</v>
       </c>
@@ -3059,7 +3063,7 @@
         <v>3.15</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>148</v>
       </c>
@@ -3097,7 +3101,7 @@
         <v>5.15</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>153</v>
       </c>
@@ -3135,7 +3139,7 @@
         <v>5.35</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="30.75">
+    <row r="37" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>58</v>
       </c>
@@ -3173,7 +3177,7 @@
         <v>8.7999999999999995E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>69</v>
       </c>
@@ -3211,7 +3215,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>161</v>
       </c>
@@ -3249,7 +3253,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>166</v>
       </c>
@@ -3287,7 +3291,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>171</v>
       </c>
@@ -3325,7 +3329,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>176</v>
       </c>
@@ -3363,7 +3367,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>181</v>
       </c>
@@ -3401,32 +3405,32 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>186</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="C44" s="32">
+      <c r="C44" s="28">
         <v>0</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="E44" s="32" t="s">
+      <c r="E44" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="F44" s="32" t="s">
+      <c r="F44" s="28" t="s">
         <v>190</v>
       </c>
-      <c r="G44" s="32">
+      <c r="G44" s="28">
         <v>2</v>
       </c>
       <c r="H44" s="1">
         <v>10</v>
       </c>
-      <c r="I44" s="32">
+      <c r="I44" s="28">
         <v>0.01</v>
       </c>
       <c r="J44" s="2">
@@ -3435,11 +3439,11 @@
       <c r="K44" s="2">
         <v>0.1</v>
       </c>
-      <c r="L44" s="32">
+      <c r="L44" s="28">
         <v>0.1</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>191</v>
       </c>

</xml_diff>